<commit_message>
Implementação de mais 2 requesitos  Changes to be committed: 	modified:   2nd Delivery/Calendario_de_Implementacao_de_Requesitos (1).xlsx
</commit_message>
<xml_diff>
--- a/2nd Delivery/Calendario_de_Implementacao_de_Requesitos (1).xlsx
+++ b/2nd Delivery/Calendario_de_Implementacao_de_Requesitos (1).xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gonçalo\Desktop\Web Progam words\Entrega dia 20\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gonçalo\Ambrosia-Board\2nd Delivery\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCE112E5-D819-4733-8BAF-568EAC695820}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6AE8EA7E-7C7F-4626-B95D-246469ED12D3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{42A9AF1C-160D-47A4-9A5D-550FA8764613}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Descrição</t>
   </si>
@@ -90,6 +90,18 @@
   </si>
   <si>
     <t>Processamento do talão do pedido</t>
+  </si>
+  <si>
+    <t>Html e Css da página da organização</t>
+  </si>
+  <si>
+    <t>Realizar toda a página da organização em html e css</t>
+  </si>
+  <si>
+    <t>Criação da funcionalidade Filtragem</t>
+  </si>
+  <si>
+    <t>Poder filtrar entre pedidos pagos, prontos, entregues</t>
   </si>
 </sst>
 </file>
@@ -164,7 +176,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -181,6 +193,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -499,7 +514,7 @@
   <dimension ref="B3:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,13 +625,30 @@
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="6"/>
+      <c r="B12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="7">
+        <v>43785</v>
+      </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="6"/>
+      <c r="B13" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="7">
+        <v>43801</v>
+      </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D3:D12">

</xml_diff>